<commit_message>
lagt inn alle tabeller mangler relationships
</commit_message>
<xml_diff>
--- a/ekstra/Databasestruktur.xlsx
+++ b/ekstra/Databasestruktur.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Orude\TeamBuilder\ekstra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\orude\TeamShare\Ekstra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3A6C1C-95C6-4A26-A274-53B857CE4B31}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="DB_struktur" sheetId="1" r:id="rId1"/>
@@ -225,7 +224,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -275,156 +274,156 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabell1" displayName="Tabell1" ref="E1:G7" totalsRowShown="0">
-  <autoFilter ref="E1:G7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabell1" displayName="Tabell1" ref="E1:G7" totalsRowShown="0">
+  <autoFilter ref="E1:G7"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Data type"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Person"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Key"/>
+    <tableColumn id="1" name="Data type"/>
+    <tableColumn id="2" name="Person"/>
+    <tableColumn id="3" name="Key"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabell2101112" displayName="Tabell2101112" ref="M15:O19" totalsRowShown="0">
-  <autoFilter ref="M15:O19" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabell2101112" displayName="Tabell2101112" ref="M15:O19" totalsRowShown="0">
+  <autoFilter ref="M15:O19"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Data type"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Gruppe"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="key"/>
+    <tableColumn id="1" name="Data type"/>
+    <tableColumn id="2" name="Gruppe"/>
+    <tableColumn id="3" name="key"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabell213" displayName="Tabell213" ref="M9:O13" totalsRowShown="0">
-  <autoFilter ref="M9:O13" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabell213" displayName="Tabell213" ref="M9:O13" totalsRowShown="0">
+  <autoFilter ref="M9:O13"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Data type"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Medlemmer"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="key"/>
+    <tableColumn id="1" name="Data type"/>
+    <tableColumn id="2" name="Medlemmer"/>
+    <tableColumn id="3" name="key"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Tabell215" displayName="Tabell215" ref="I3:K6" totalsRowShown="0">
-  <autoFilter ref="I3:K6" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabell215" displayName="Tabell215" ref="I3:K6" totalsRowShown="0">
+  <autoFilter ref="I3:K6"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Data type"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Deltakertype"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="key"/>
+    <tableColumn id="1" name="Data type"/>
+    <tableColumn id="2" name="Deltakertype"/>
+    <tableColumn id="3" name="key"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Tabell21011" displayName="Tabell21011" ref="Q9:S12" totalsRowShown="0">
-  <autoFilter ref="Q9:S12" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabell21011" displayName="Tabell21011" ref="Q9:S12" totalsRowShown="0">
+  <autoFilter ref="Q9:S12"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Data type"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Join level"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="key"/>
+    <tableColumn id="1" name="Data type"/>
+    <tableColumn id="2" name="Join level"/>
+    <tableColumn id="3" name="key"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabell3" displayName="Tabell3" ref="A1:C3" totalsRowShown="0">
-  <autoFilter ref="A1:C3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabell3" displayName="Tabell3" ref="A1:C3" totalsRowShown="0">
+  <autoFilter ref="A1:C3"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Data type"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Postadresse"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Key"/>
+    <tableColumn id="1" name="Data type"/>
+    <tableColumn id="2" name="Postadresse"/>
+    <tableColumn id="3" name="Key"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabell4" displayName="Tabell4" ref="A14:C17" totalsRowShown="0">
-  <autoFilter ref="A14:C17" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabell4" displayName="Tabell4" ref="A14:C17" totalsRowShown="0">
+  <autoFilter ref="A14:C17"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Data type"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="AccessLevel"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Key"/>
+    <tableColumn id="1" name="Data type"/>
+    <tableColumn id="2" name="AccessLevel"/>
+    <tableColumn id="3" name="Key"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabell5" displayName="Tabell5" ref="A9:C12" totalsRowShown="0">
-  <autoFilter ref="A9:C12" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabell5" displayName="Tabell5" ref="A9:C12" totalsRowShown="0">
+  <autoFilter ref="A9:C12"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Data type"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Tittler"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Key"/>
+    <tableColumn id="1" name="Data type"/>
+    <tableColumn id="2" name="Tittler"/>
+    <tableColumn id="3" name="Key"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabell6" displayName="Tabell6" ref="E9:G16" totalsRowShown="0">
-  <autoFilter ref="E9:G16" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabell6" displayName="Tabell6" ref="E9:G16" totalsRowShown="0">
+  <autoFilter ref="E9:G16"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Data type"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="User"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="key"/>
+    <tableColumn id="1" name="Data type"/>
+    <tableColumn id="2" name="User"/>
+    <tableColumn id="3" name="key"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tabell7" displayName="Tabell7" ref="A19:C25" totalsRowShown="0">
-  <autoFilter ref="A19:C25" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabell7" displayName="Tabell7" ref="A19:C25" totalsRowShown="0">
+  <autoFilter ref="A19:C25"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Data type"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Innlegg"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="key"/>
+    <tableColumn id="1" name="Data type"/>
+    <tableColumn id="2" name="Innlegg"/>
+    <tableColumn id="3" name="key"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabell8" displayName="Tabell8" ref="E19:G22" totalsRowShown="0">
-  <autoFilter ref="E19:G22" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabell8" displayName="Tabell8" ref="E19:G22" totalsRowShown="0">
+  <autoFilter ref="E19:G22"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Data type"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="User_posts"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="key"/>
+    <tableColumn id="1" name="Data type"/>
+    <tableColumn id="2" name="User_posts"/>
+    <tableColumn id="3" name="key"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabell2" displayName="Tabell2" ref="I9:K14" totalsRowShown="0">
-  <autoFilter ref="I9:K14" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabell2" displayName="Tabell2" ref="I9:K14" totalsRowShown="0">
+  <autoFilter ref="I9:K14"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Data type"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Deltaker"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="key"/>
+    <tableColumn id="1" name="Data type"/>
+    <tableColumn id="2" name="Deltaker"/>
+    <tableColumn id="3" name="key"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Tabell210" displayName="Tabell210" ref="I17:K22" totalsRowShown="0">
-  <autoFilter ref="I17:K22" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabell210" displayName="Tabell210" ref="I17:K22" totalsRowShown="0">
+  <autoFilter ref="I17:K22"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Data type"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Omrade"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="key"/>
+    <tableColumn id="1" name="Data type"/>
+    <tableColumn id="2" name="Omrade"/>
+    <tableColumn id="3" name="key"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -726,37 +725,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.81640625" customWidth="1"/>
-    <col min="9" max="9" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.81640625" customWidth="1"/>
-    <col min="13" max="13" width="13.54296875" customWidth="1"/>
-    <col min="14" max="14" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.54296875" customWidth="1"/>
-    <col min="17" max="17" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.5703125" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -779,7 +778,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -802,7 +801,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -828,7 +827,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>29</v>
       </c>
@@ -845,7 +844,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>29</v>
       </c>
@@ -865,7 +864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>29</v>
       </c>
@@ -882,7 +881,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>28</v>
       </c>
@@ -899,12 +898,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="V8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -954,7 +953,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1004,7 +1003,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1051,7 +1050,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1095,7 +1094,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>29</v>
       </c>
@@ -1127,7 +1126,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1153,7 +1152,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1182,7 +1181,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1208,7 +1207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1231,7 +1230,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I18" t="s">
         <v>28</v>
       </c>
@@ -1251,7 +1250,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1283,7 +1282,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1309,7 +1308,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1332,7 +1331,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1355,7 +1354,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1363,7 +1362,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1371,7 +1370,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Løste forgein key, klar til å legge inn og gjøre ferdig databasen
</commit_message>
<xml_diff>
--- a/ekstra/Databasestruktur.xlsx
+++ b/ekstra/Databasestruktur.xlsx
@@ -728,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>